<commit_message>
Modularised to use promises
</commit_message>
<xml_diff>
--- a/data/training-set.xlsx
+++ b/data/training-set.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="460" windowWidth="24600" windowHeight="15540" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="1000" yWindow="460" windowWidth="24600" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Pretty" sheetId="1" r:id="rId1"/>
@@ -394,7 +394,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H104"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5656,9 +5656,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
-    </sheetView>
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>